<commit_message>
Hotfix: Wed Oct 16 17:38:15 RTZ 2024
</commit_message>
<xml_diff>
--- a/files/database_tables.xlsx
+++ b/files/database_tables.xlsx
@@ -635,7 +635,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D32"/>
+  <dimension ref="A1:D37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1219,6 +1219,245 @@
         print(e)
 if __name__ == '__main__':
     create_tables()</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>2094</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Скрипт удаления из таблицы баз данных определенных id </t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Скрипт удаления из таблицы баз данных определенных id </t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t># Подключаем библиотеку sqlite3
+import sqlite3
+# Подключаемся в базе данных
+con = sqlite3.connect("../database1.db")
+cur = con.cursor()
+res = cur.execute("DELETE FROM links WHERE id IN (12,13,14)")
+res.fetchall()
+con.commit()</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>2095</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Скрипт очистки таблицы базы данных</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>Скрипт очистки таблицы базы данных</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>import sqlite3
+con = sqlite3.connect("/database1.db")
+cur = con.cursor()
+res = cur.execute("DROP TABLE table_name")
+con.commit()</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>2096</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Скрипт удаления таблицы</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>Скрипт удаления таблицы</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>import sqlite3
+con = sqlite3.connect("/database1.db")
+cur = con.cursor()
+res = cur.execute("DROP TABLE table_name")
+con.commit()</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>2097</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Скрипт вставки значений в таблицу</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>Скрипт вставки значений в таблицу</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t xml:space="preserve"># Подключаем библиотеку sqlite3
+import sqlite3
+# Подключаемся в базе данных
+con = sqlite3.connect("../database1.db")
+cur = con.cursor()
+data = (
+    {"id": None, "name": "test", "link": "test"},
+    {"id": None, "name": "test", "link": "test"},
+    {"id": None, "name": "test", "link": "test"},
+)
+cur.executemany("INSERT INTO links VALUES(:id,:name, :link)", data)
+con.commit()
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>2098</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Экземпляр приложения Flask</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>Экземпляр приложения Flask с подключением внешней базы данных и пагинацией</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>import flask
+import pymysql.cursors
+from flask_paginate import Pagination, get_page_args
+app = flask.Flask(__name__)
+app.secret_key = "secret key"
+@app.errorhandler(404)
+def page_not_found(e):
+    return flask.render_template('404.html'), 404
+def get_db_connection():
+    conn = pymysql.connect(host='localhost',
+                           port=3307,
+                           user='root',
+                           password='1',
+                           database='test_base',
+                           charset='utf8',
+                           cursorclass=pymysql.cursors.DictCursor)
+    return conn
+def close_db_connection(conn):
+    conn.close()
+@app.route("/")
+def index():
+    conn = get_db_connection()
+    with conn.cursor() as cur:
+        cur.execute("SELECT * FROM test_table")
+        test_list_posts = cur.fetchall()
+    conn.close()
+    page, per_page, offset = get_page_args(page_parameter='page',
+                                           per_page_parameter='per_page')
+    total = len(test_list_posts)
+    def get_test_list_posts(offset=0, per_page=5):
+        return test_list_posts[offset: offset + per_page]
+    pagination_test_list_posts = get_test_list_posts(offset=offset, per_page=per_page)
+    pagination = Pagination(page=page, per_page=per_page, total=total,
+                        css_framework='bootstrap4',
+                        display_msg="Показано &lt;b&gt;{start} - {end}&lt;/b&gt; {record_name} из &lt;b&gt;{total}&lt;/b&gt;",
+                        record_name="записей")
+    return flask.render_template("test/test_list_posts.html",
+                                 test_list_posts=pagination_test_list_posts, 
+                                                            page=page,
+                           per_page=per_page,
+                           pagination=pagination,)
+@app.route("/view/&lt;int:test_id&gt;")
+def get_post_test_post(test_id):
+    conn = get_db_connection()
+    with conn.cursor() as cur:
+        sql = "SELECT * FROM `test_table` WHERE `test_id` =%s"
+        cur.execute(sql, test_id)
+        test_view_post = cur.fetchone()
+    conn.close()
+    return flask.render_template("test/test_view_post.html",
+                                 test_view_post=test_view_post, )
+@app.route("/edit/&lt;int:test_id&gt;/", methods=("GET", "POST"))
+def edit_test_post(test_id):
+    conn = get_db_connection()
+    with conn.cursor() as cur:
+        sql = "SELECT * FROM `test_table` WHERE `test_id` =%s"
+        cur.execute(sql, (test_id,))
+        edit_test_view = cur.fetchone()
+    if flask.request.method == "POST":
+        test_edit_post_text = flask.request.form["test_text"]
+        if len(flask.request.form['test_text']) &gt; 1:
+            conn = get_db_connection()
+            with conn.cursor() as cur:
+                sql = "UPDATE `test_table` SET `test_text` =%s  WHERE `test_id` =%s"
+                cur.execute(
+                    sql, (test_edit_post_text, test_id),
+                )
+            conn.commit()
+            conn.close()
+            if not test_edit_post_text:
+                flask.flash('Ошибка сохранения записи, вы ввели мало символов!', category='error')
+            else:
+                flask.flash('Запись успешно сохранена!', category='success')
+            # В случае соблюдения условий заполнения полей, произойдёт перенаправление
+            return flask.redirect(flask.url_for("index"))
+        else:
+            flask.flash('Ошибка сохранения записи!', category='error')
+    return flask.render_template("test/edit_test_post.html", edit_test_view=edit_test_view)
+@app.route("/new_post", methods=["GET", "POST"])
+def add_test_post():
+    if flask.request.method == "POST":
+        new_test_post = flask.request.form["test_text"]
+        if len(flask.request.form['test_text']) &gt; 1:
+            conn = get_db_connection()
+            with conn.cursor() as cur:
+                sql = "INSERT INTO `test_table` (`test_text`) VALUES (%s)"
+                cur.execute(
+                    sql, new_test_post,
+                )
+            conn.commit()
+            conn.close()
+            if not new_test_post:
+                flask.flash('Ошибка сохранения записи, Вы ввели слишком мало символов!', category='error')
+            else:
+                flask.flash('Запись успешно добавлена!')
+            # В случае соблюдения условий заполнения полей, произойдёт перенаправление
+            return flask.redirect(flask.url_for("index"))
+        else:
+            flask.flash('Ошибка сохранения записи!', category='error')
+    return flask.render_template("test/add_test_post.html")
+@app.route("/delete/&lt;int:test_id&gt;/", methods=("POST",))
+def delete_post_test(test_id):
+    conn = get_db_connection()
+    with conn.cursor() as cur:
+        sql = "DELETE FROM `test_table` WHERE `test_id` =%s"
+        cur.execute(
+            sql, test_id,
+        )
+    conn.commit()
+    conn.close()
+    return flask.redirect(flask.url_for("index"))
+if __name__ == "__main__":
+    app.run(debug=True, host='0.0.0.0', port=83)</t>
         </is>
       </c>
     </row>
@@ -1480,7 +1719,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C66"/>
+  <dimension ref="A1:C70"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2478,6 +2717,87 @@
         </is>
       </c>
     </row>
+    <row r="67">
+      <c r="A67" t="n">
+        <v>97</v>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>#!/bin/commands
+rm -rf ~/Downloads
+mkdir ~/Downloads</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Скрипт для удаления папки и её создания
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="n">
+        <v>98</v>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t xml:space="preserve">#!/bin/bash 
+# Задаем переменную DATE, в переменной указываем команду date (для вывода даты и времени) 
+DATE=$(date) 
+# Задаем переменную TEXT, в переменной указываем текст коммита и добавляем ранее добавленную переменную 
+DATE TEXT="Add commit date: $DATE" 
+# Добавляем файлы для коммита 
+git add . 
+# Объявляем коммит с созданной ранее переменной TEXT 
+git commit -m "$TEXT" 
+# Отправляем коммит на репозиторий 
+git push </t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t xml:space="preserve">bash-скрипт для формирования коммита и отправки его на репозиторий с указанием даты 
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="n">
+        <v>99</v>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>#!/bin/bash
+# Запускается 1-е приложение следующим скриптом. Указывается путь исполняемой программы и путь к самому приложению.
+~/AppData/Local/Programs/Python/Python312/python.exe ~/flask-mysql-project/app.py &amp;
+# Затем запускается 2-е приложение
+~/AppData/Local/Programs/Python/Python312/python.exe /p/s.savin/flask-base/app.py &amp;
+# И наконец запускается 3-е приложение
+~/AppData/Local/Programs/Python/Python312/python.exe /p/s.savin/flask-project-full/app.py &amp;</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t xml:space="preserve">bash-скрипт который запускает три приложения flask
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="n">
+        <v>100</v>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>sfsdfdsfsdfsdfsd</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>sdfsdfsdfsdfsdfsdfsd</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Hotfix: Thu Oct 17 17:53:35 RTZ 2024
</commit_message>
<xml_diff>
--- a/files/database_tables.xlsx
+++ b/files/database_tables.xlsx
@@ -635,7 +635,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D37"/>
+  <dimension ref="A1:D38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1461,6 +1461,26 @@
         </is>
       </c>
     </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>2099</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Тестовая запись</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>Тестовая запись</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>Тестовая запись</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -1719,7 +1739,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C70"/>
+  <dimension ref="A1:C71"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2785,16 +2805,32 @@
     </row>
     <row r="70">
       <c r="A70" t="n">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>sfsdfdsfsdfsdfsd</t>
+          <t>#!/bin/bash
+venv/Scripts/python.exe app.py &amp;</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>sdfsdfsdfsdfsdfsdfsd</t>
+          <t>Тестовая bash команда</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="n">
+        <v>105</v>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>delete_bash_command</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>delete_bash_command</t>
         </is>
       </c>
     </row>

</xml_diff>